<commit_message>
add MTK for isp7
</commit_message>
<xml_diff>
--- a/MTK/AF/AF_Cali/face_roi.xlsx
+++ b/MTK/AF/AF_Cali/face_roi.xlsx
@@ -1,23 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\ADB\MTK\AF\AF_Cali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C1854D-4A9D-4BB3-9D02-C6B4DACA3957}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2117117-EA44-4EB8-AD9B-3C9CC60FC859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18645" yWindow="-16455" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -562,7 +572,7 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -625,60 +635,60 @@
         <v>15</v>
       </c>
       <c r="B2" s="5">
-        <v>1098</v>
+        <v>1361</v>
       </c>
       <c r="C2" s="5">
-        <v>915</v>
+        <v>1453</v>
       </c>
       <c r="D2" s="5">
-        <v>160</v>
+        <v>518</v>
       </c>
       <c r="E2" s="5">
-        <v>201</v>
+        <v>376</v>
       </c>
       <c r="F2" s="1">
         <f>B2</f>
-        <v>1098</v>
+        <v>1361</v>
       </c>
       <c r="G2" s="1">
         <f>C2</f>
-        <v>915</v>
+        <v>1453</v>
       </c>
       <c r="H2" s="1">
         <f>B2+D2</f>
-        <v>1258</v>
+        <v>1879</v>
       </c>
       <c r="I2" s="1">
         <f>C2</f>
-        <v>915</v>
+        <v>1453</v>
       </c>
       <c r="J2" s="1">
         <f>B2</f>
-        <v>1098</v>
+        <v>1361</v>
       </c>
       <c r="K2" s="1">
         <f>C2+E2</f>
-        <v>1116</v>
+        <v>1829</v>
       </c>
       <c r="L2" s="1">
         <f>B2+D2</f>
-        <v>1258</v>
+        <v>1879</v>
       </c>
       <c r="M2" s="10">
         <f>C2+E2</f>
-        <v>1116</v>
+        <v>1829</v>
       </c>
       <c r="N2" s="11">
         <f>D4*E4/D2/E2</f>
-        <v>0.87468905472636815</v>
+        <v>0.58703688490922534</v>
       </c>
       <c r="O2" s="12">
         <f>ABS($B$3-$B$2)/D2</f>
-        <v>8.7499999999999994E-2</v>
+        <v>0.2335907335907336</v>
       </c>
       <c r="P2" s="14">
         <f>ABS($C$3-$C$2)/E2</f>
-        <v>1.4925373134328358E-2</v>
+        <v>0.23404255319148937</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.15">
@@ -686,60 +696,60 @@
         <v>16</v>
       </c>
       <c r="B3" s="5">
-        <v>1084</v>
+        <v>1482</v>
       </c>
       <c r="C3" s="5">
-        <v>918</v>
+        <v>1541</v>
       </c>
       <c r="D3" s="5">
-        <v>159</v>
+        <v>450</v>
       </c>
       <c r="E3" s="5">
-        <v>194</v>
+        <v>349</v>
       </c>
       <c r="F3" s="1">
         <f>B3</f>
-        <v>1084</v>
+        <v>1482</v>
       </c>
       <c r="G3" s="1">
         <f>C3</f>
-        <v>918</v>
+        <v>1541</v>
       </c>
       <c r="H3" s="1">
         <f>B3+D3</f>
-        <v>1243</v>
+        <v>1932</v>
       </c>
       <c r="I3" s="1">
         <f>C3</f>
-        <v>918</v>
+        <v>1541</v>
       </c>
       <c r="J3" s="1">
         <f>B3</f>
-        <v>1084</v>
+        <v>1482</v>
       </c>
       <c r="K3" s="1">
         <f>C3+E3</f>
-        <v>1112</v>
+        <v>1890</v>
       </c>
       <c r="L3" s="1">
         <f>B3+D3</f>
-        <v>1243</v>
+        <v>1932</v>
       </c>
       <c r="M3" s="10">
         <f>C3+E3</f>
-        <v>1112</v>
+        <v>1890</v>
       </c>
       <c r="N3" s="11">
         <f>D4*E4/D3/E3</f>
-        <v>0.91194968553459121</v>
+        <v>0.72802292263610324</v>
       </c>
       <c r="O3" s="12">
         <f>ABS($B$3-$B$2)/D3</f>
-        <v>8.8050314465408799E-2</v>
+        <v>0.2688888888888889</v>
       </c>
       <c r="P3" s="14">
         <f>ABS($C$3-$C$2)/E3</f>
-        <v>1.5463917525773196E-2</v>
+        <v>0.25214899713467048</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.15">
@@ -748,51 +758,51 @@
       </c>
       <c r="B4" s="1">
         <f>F4</f>
-        <v>1098</v>
+        <v>1482</v>
       </c>
       <c r="C4" s="1">
         <f>G4</f>
-        <v>918</v>
+        <v>1541</v>
       </c>
       <c r="D4" s="1">
         <f>H4-F4</f>
-        <v>145</v>
+        <v>397</v>
       </c>
       <c r="E4" s="1">
         <f>K4-G4</f>
-        <v>194</v>
+        <v>288</v>
       </c>
       <c r="F4" s="1">
         <f>(IF(H3&lt;F2,F2,IF(F3&gt;H2,F2,IF(F3&lt;F2,F2,F3))))</f>
-        <v>1098</v>
+        <v>1482</v>
       </c>
       <c r="G4" s="1">
         <f>(IF(K3&lt;G2,G2,IF(G3&gt;K2,G2,IF(G3&lt;G2,G2,G3))))</f>
-        <v>918</v>
+        <v>1541</v>
       </c>
       <c r="H4" s="1">
         <f>L4</f>
-        <v>1243</v>
+        <v>1879</v>
       </c>
       <c r="I4" s="1">
         <f>G4</f>
-        <v>918</v>
+        <v>1541</v>
       </c>
       <c r="J4" s="1">
         <f>G4</f>
-        <v>918</v>
+        <v>1541</v>
       </c>
       <c r="K4" s="1">
         <f>M4</f>
-        <v>1112</v>
+        <v>1829</v>
       </c>
       <c r="L4" s="1">
         <f>IF(L3&lt;F2,L2,IF(F3&gt;L2,L2,IF(L3&lt;L2,L3,L2)))</f>
-        <v>1243</v>
+        <v>1879</v>
       </c>
       <c r="M4" s="10">
         <f>IF(M3&lt;G2,M2,IF(G3&gt;M2,M2,IF(M3&lt;M2,M3,M2)))</f>
-        <v>1112</v>
+        <v>1829</v>
       </c>
       <c r="N4" s="13"/>
     </row>

</xml_diff>